<commit_message>
corrected lat lon format and removed ZPL sensors not deployed
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GA02HYPM_00002.xlsx
+++ b/deployment/Omaha_Cal_Info_GA02HYPM_00002.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="71">
   <si>
     <t>Ref Des</t>
   </si>
@@ -160,12 +160,6 @@
     <t>GA02HYPM-00002</t>
   </si>
   <si>
-    <t>42° 58.850’ S</t>
-  </si>
-  <si>
-    <t>42° 32.515’ W</t>
-  </si>
-  <si>
     <t>NBP-15-10</t>
   </si>
   <si>
@@ -199,9 +193,6 @@
     <t>14880</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Not Deployed</t>
   </si>
   <si>
@@ -248,6 +239,12 @@
   </si>
   <si>
     <t>OL000059</t>
+  </si>
+  <si>
+    <t>42° 58.850' S</t>
+  </si>
+  <si>
+    <t>42° 32.515' W</t>
   </si>
 </sst>
 </file>
@@ -1845,8 +1842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1870,7 +1867,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1908,7 +1905,7 @@
     </row>
     <row r="2" spans="1:14" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>40</v>
@@ -1927,20 +1924,26 @@
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="16" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="J2" s="16">
         <v>5196</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L2" s="2"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
+      <c r="M2" s="18">
+        <f>((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="N",1,-1))</f>
+        <v>-42.980833333333337</v>
+      </c>
+      <c r="N2" s="18">
+        <f>((LEFT(I2,(FIND("°",I2,1)-1)))+(MID(I2,(FIND("°",I2,1)+1),(FIND("'",I2,1))-(FIND("°",I2,1)+1))/60))*(IF(RIGHT(I2,1)="E",1,-1))</f>
+        <v>-42.541916666666665</v>
+      </c>
     </row>
     <row r="3" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E3" s="19"/>
@@ -2013,10 +2016,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2024,12 +2027,12 @@
     <col min="1" max="1" width="34.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="78.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" style="1" customWidth="1"/>
     <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
@@ -2038,7 +2041,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>1</v>
@@ -2047,7 +2050,7 @@
         <v>24</v>
       </c>
       <c r="E1" s="36" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>2</v>
@@ -2068,7 +2071,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>41</v>
@@ -2077,7 +2080,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F3" s="33">
         <v>4015</v>
@@ -2097,7 +2100,7 @@
         <v>30</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>41</v>
@@ -2106,7 +2109,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F4" s="33">
         <v>4015</v>
@@ -2123,7 +2126,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>41</v>
@@ -2132,7 +2135,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F5" s="33">
         <v>4015</v>
@@ -2149,7 +2152,7 @@
         <v>30</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>41</v>
@@ -2158,7 +2161,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F6" s="33">
         <v>4015</v>
@@ -2175,7 +2178,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>41</v>
@@ -2184,7 +2187,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F7" s="33">
         <v>4015</v>
@@ -2204,7 +2207,7 @@
         <v>30</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>41</v>
@@ -2213,7 +2216,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F8" s="33">
         <v>4015</v>
@@ -2233,7 +2236,7 @@
         <v>30</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>41</v>
@@ -2242,7 +2245,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F9" s="33">
         <v>4015</v>
@@ -2262,7 +2265,7 @@
         <v>30</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>41</v>
@@ -2271,7 +2274,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F10" s="33">
         <v>4015</v>
@@ -2296,16 +2299,16 @@
         <v>32</v>
       </c>
       <c r="B12" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="24" t="s">
         <v>58</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="1">
-        <v>2</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>61</v>
       </c>
       <c r="F12" s="28">
         <v>2197</v>
@@ -2325,16 +2328,16 @@
         <v>32</v>
       </c>
       <c r="B13" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2</v>
+      </c>
+      <c r="E13" s="24" t="s">
         <v>58</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="1">
-        <v>2</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>61</v>
       </c>
       <c r="F13" s="28">
         <v>2197</v>
@@ -2356,7 +2359,7 @@
         <v>33</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>41</v>
@@ -2365,7 +2368,7 @@
         <v>2</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F15" s="28">
         <v>152</v>
@@ -2382,7 +2385,7 @@
         <v>33</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>41</v>
@@ -2391,7 +2394,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F16" s="28">
         <v>152</v>
@@ -2413,7 +2416,7 @@
         <v>34</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>41</v>
@@ -2422,7 +2425,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F18" s="28">
         <v>1255</v>
@@ -2439,7 +2442,7 @@
         <v>34</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>41</v>
@@ -2448,7 +2451,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F19" s="28">
         <v>1255</v>
@@ -2470,7 +2473,7 @@
         <v>35</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>41</v>
@@ -2479,7 +2482,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F21" s="28">
         <v>4016</v>
@@ -2499,7 +2502,7 @@
         <v>35</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>41</v>
@@ -2508,7 +2511,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F22" s="28">
         <v>4016</v>
@@ -2525,7 +2528,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>41</v>
@@ -2534,7 +2537,7 @@
         <v>2</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F23" s="28">
         <v>4016</v>
@@ -2551,7 +2554,7 @@
         <v>35</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>41</v>
@@ -2560,7 +2563,7 @@
         <v>2</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F24" s="28">
         <v>4016</v>
@@ -2577,7 +2580,7 @@
         <v>35</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>41</v>
@@ -2586,7 +2589,7 @@
         <v>2</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F25" s="28">
         <v>4016</v>
@@ -2606,7 +2609,7 @@
         <v>35</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>41</v>
@@ -2615,7 +2618,7 @@
         <v>2</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F26" s="28">
         <v>4016</v>
@@ -2635,7 +2638,7 @@
         <v>35</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>41</v>
@@ -2644,7 +2647,7 @@
         <v>2</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F27" s="28">
         <v>4016</v>
@@ -2664,7 +2667,7 @@
         <v>35</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>41</v>
@@ -2673,7 +2676,7 @@
         <v>2</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F28" s="28">
         <v>4016</v>
@@ -2698,7 +2701,7 @@
         <v>37</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>41</v>
@@ -2707,7 +2710,7 @@
         <v>2</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F30" s="28">
         <v>2196</v>
@@ -2724,7 +2727,7 @@
         <v>37</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>41</v>
@@ -2733,7 +2736,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F31" s="28">
         <v>2196</v>
@@ -2750,12 +2753,12 @@
       <c r="G32" s="27"/>
       <c r="H32" s="27"/>
     </row>
-    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>41</v>
@@ -2764,7 +2767,7 @@
         <v>2</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F33" s="28">
         <v>153</v>
@@ -2776,12 +2779,12 @@
         <v>-42.980833333333337</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="26" t="s">
         <v>38</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>41</v>
@@ -2790,7 +2793,7 @@
         <v>2</v>
       </c>
       <c r="E34" s="24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F34" s="28">
         <v>153</v>
@@ -2802,17 +2805,17 @@
         <v>-42.541916666666665</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F35" s="27"/>
       <c r="G35" s="27"/>
       <c r="H35" s="27"/>
     </row>
-    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>41</v>
@@ -2821,7 +2824,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F36" s="28">
         <v>1254</v>
@@ -2833,12 +2836,12 @@
         <v>-42.980833333333337</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
         <v>39</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>41</v>
@@ -2847,7 +2850,7 @@
         <v>2</v>
       </c>
       <c r="E37" s="24" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F37" s="28">
         <v>1254</v>
@@ -2859,74 +2862,64 @@
         <v>-42.541916666666665</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F38" s="27"/>
       <c r="G38" s="27"/>
       <c r="H38" s="27"/>
     </row>
-    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D39" s="1">
-        <v>2</v>
-      </c>
-      <c r="F39" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="G39" s="27"/>
-      <c r="H39" s="27"/>
+    <row r="39" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="I39" s="24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="27"/>
-    </row>
-    <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B41" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D41" s="1">
-        <v>2</v>
-      </c>
-      <c r="E41" s="24"/>
-      <c r="F41" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="G41" s="27"/>
-      <c r="H41" s="27"/>
+        <v>53</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K39" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O39" s="31"/>
+      <c r="P39" s="27"/>
+      <c r="Q39" s="27"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O40" s="27"/>
+      <c r="P40" s="27"/>
+      <c r="Q40" s="27"/>
+    </row>
+    <row r="41" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="I41" s="24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K41" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N41" s="24"/>
+      <c r="O41" s="31"/>
+      <c r="P41" s="27"/>
+      <c r="Q41" s="27"/>
+    </row>
+    <row r="42" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="B42" s="24"/>
       <c r="E42" s="24"/>
       <c r="F42" s="27"/>
       <c r="G42" s="27"/>
       <c r="H42" s="27"/>
     </row>
-    <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B43" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>41</v>
@@ -2935,10 +2928,10 @@
         <v>2</v>
       </c>
       <c r="E43" s="24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F43" s="28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G43" s="27" t="s">
         <v>5</v>
@@ -2948,12 +2941,12 @@
       </c>
       <c r="I43" s="23"/>
     </row>
-    <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>41</v>
@@ -2962,10 +2955,10 @@
         <v>2</v>
       </c>
       <c r="E44" s="24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F44" s="28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G44" s="27" t="s">
         <v>6</v>
@@ -2975,12 +2968,12 @@
       </c>
       <c r="I44" s="23"/>
     </row>
-    <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>41</v>
@@ -2989,10 +2982,10 @@
         <v>2</v>
       </c>
       <c r="E45" s="24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F45" s="28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G45" s="27" t="s">
         <v>7</v>
@@ -3002,19 +2995,19 @@
       </c>
       <c r="I45" s="23"/>
     </row>
-    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="B46" s="24"/>
       <c r="E46" s="24"/>
       <c r="F46" s="27"/>
       <c r="G46" s="27"/>
       <c r="H46" s="27"/>
     </row>
-    <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B47" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>41</v>
@@ -3023,21 +3016,21 @@
         <v>2</v>
       </c>
       <c r="E47" s="24" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F47" s="29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G47" s="30"/>
       <c r="H47" s="30"/>
       <c r="I47" s="23"/>
     </row>
-    <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>41</v>
@@ -3046,10 +3039,10 @@
         <v>2</v>
       </c>
       <c r="E48" s="24" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F48" s="29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G48" s="27"/>
       <c r="H48" s="27"/>
@@ -3057,10 +3050,10 @@
     </row>
     <row r="49" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B49" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>41</v>
@@ -3069,10 +3062,10 @@
         <v>2</v>
       </c>
       <c r="E49" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F49" s="29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G49" s="27"/>
       <c r="H49" s="27"/>

</xml_diff>